<commit_message>
CL 0 -> CL 1 test_gap_9서9 collision 1
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum Yes ob 0_0/Curriculum Yes ob 0_0_TEST_TRAIN/Curriculum Yes ob 0_0_TEST_TRAIN_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum Yes ob 0_0/Curriculum Yes ob 0_0_TEST_TRAIN/Curriculum Yes ob 0_0_TEST_TRAIN_Test_Result.xlsx
@@ -445,16 +445,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>